<commit_message>
Add english text to pie chart
</commit_message>
<xml_diff>
--- a/docs/01-basics/pie-chart-overview.xlsx
+++ b/docs/01-basics/pie-chart-overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/Documents/developer/github_isaqb/advanced-template/docs/01-basics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9EEE5A9-4662-B94B-B2FD-B2F617332F37}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B0021D-F328-FD4D-84C2-7CEE7CC41D66}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6180" yWindow="1900" windowWidth="24560" windowHeight="17660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,16 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
-  <si>
-    <t>Examples</t>
-  </si>
-  <si>
-    <t>Design and development</t>
-  </si>
-  <si>
-    <t>Specification and communication</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Vortrag</t>
   </si>
@@ -54,12 +45,6 @@
   </si>
   <si>
     <t>Gesamt</t>
-  </si>
-  <si>
-    <t>Basic concepts of software architecture</t>
-  </si>
-  <si>
-    <t>Software architecture and quality</t>
   </si>
   <si>
     <t>Thema mit Einleitung</t>
@@ -78,6 +63,24 @@
   </si>
   <si>
     <t>Thema mit Abschlussbeispiel</t>
+  </si>
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <t>xz</t>
+  </si>
+  <si>
+    <t>Lots of theory</t>
+  </si>
+  <si>
+    <t>xy and example</t>
+  </si>
+  <si>
+    <t>abc and d</t>
+  </si>
+  <si>
+    <t>final example</t>
   </si>
 </sst>
 </file>
@@ -696,47 +699,53 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'EN-Graphic'!$A$1:$A$5</c:f>
+              <c:f>'EN-Graphic'!$A$1:$A$6</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>Basic concepts of software architecture</c:v>
+                  <c:v>Introduction</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Design and development</c:v>
+                  <c:v>xz</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Specification and communication</c:v>
+                  <c:v>Lots of theory</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Software architecture and quality</c:v>
+                  <c:v>xy and example</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Examples</c:v>
+                  <c:v>abc and d</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>final example</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'EN-Graphic'!$B$1:$B$5</c:f>
+              <c:f>'EN-Graphic'!$B$1:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>120</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>390</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>240</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>90</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>60</c:v>
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>120</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1192,103 +1201,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1">
-        <v>180</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2">
-        <v>150</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3">
-        <v>120</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>180</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5">
-        <v>210</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6">
-        <v>120</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B7">
-        <f>SUM(B1:B6)</f>
-        <v>960</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="C1" sqref="C1:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1299,48 +1215,131 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B1">
-        <v>120</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2">
-        <v>390</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>240</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
+      <c r="B5">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <f>SUM(B1:B6)</f>
+        <v>960</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
       <c r="B4">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>0</v>
+      <c r="A5" t="s">
+        <v>13</v>
       </c>
       <c r="B5">
-        <v>60</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B6">
-        <f>SUM(B1:B5)</f>
-        <v>900</v>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <f>SUM(B1:B6)</f>
+        <v>960</v>
       </c>
     </row>
   </sheetData>
@@ -1361,13 +1360,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update fonts in XLS for image export
</commit_message>
<xml_diff>
--- a/docs/01-basics/pie-chart-overview.xlsx
+++ b/docs/01-basics/pie-chart-overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/Documents/developer/github_isaqb/advanced-template/docs/01-basics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B0021D-F328-FD4D-84C2-7CEE7CC41D66}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09173C1-5A8A-9F47-8274-D52D978FC160}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="1900" windowWidth="24560" windowHeight="17660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6180" yWindow="1900" windowWidth="24560" windowHeight="17660" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DE-Grafik" sheetId="3" r:id="rId1"/>
@@ -158,11 +158,13 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:explosion val="19"/>
+          <c:spPr>
+            <a:effectLst/>
+          </c:spPr>
+          <c:explosion val="4"/>
           <c:dPt>
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="7"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000000-A4C3-CF4A-A4D5-5E2A8878AA85}"/>
@@ -172,7 +174,6 @@
           <c:dPt>
             <c:idx val="1"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="5"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-A4C3-CF4A-A4D5-5E2A8878AA85}"/>
@@ -182,7 +183,6 @@
           <c:dPt>
             <c:idx val="2"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="7"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000002-A4C3-CF4A-A4D5-5E2A8878AA85}"/>
@@ -192,7 +192,6 @@
           <c:dPt>
             <c:idx val="3"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="6"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-A4C3-CF4A-A4D5-5E2A8878AA85}"/>
@@ -202,7 +201,6 @@
           <c:dPt>
             <c:idx val="4"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="8"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000004-A4C3-CF4A-A4D5-5E2A8878AA85}"/>
@@ -212,7 +210,6 @@
           <c:dPt>
             <c:idx val="5"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="7"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-A4C3-CF4A-A4D5-5E2A8878AA85}"/>
@@ -456,7 +453,10 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="1800"/>
+        <a:defRPr sz="1400">
+          <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+          <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="de-DE"/>
     </a:p>
@@ -491,11 +491,13 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:explosion val="19"/>
+          <c:spPr>
+            <a:effectLst/>
+          </c:spPr>
+          <c:explosion val="4"/>
           <c:dPt>
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="7"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000000-01D3-8347-BAD4-8610D9832016}"/>
@@ -505,7 +507,6 @@
           <c:dPt>
             <c:idx val="1"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="5"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-01D3-8347-BAD4-8610D9832016}"/>
@@ -515,7 +516,6 @@
           <c:dPt>
             <c:idx val="2"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="7"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000002-01D3-8347-BAD4-8610D9832016}"/>
@@ -525,7 +525,6 @@
           <c:dPt>
             <c:idx val="3"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="6"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-01D3-8347-BAD4-8610D9832016}"/>
@@ -535,7 +534,6 @@
           <c:dPt>
             <c:idx val="4"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="8"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000004-01D3-8347-BAD4-8610D9832016}"/>
@@ -545,7 +543,6 @@
           <c:dPt>
             <c:idx val="5"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="7"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-01D3-8347-BAD4-8610D9832016}"/>
@@ -782,7 +779,10 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="1600"/>
+        <a:defRPr sz="1400">
+          <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+          <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="de-DE"/>
     </a:p>
@@ -1203,8 +1203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C6"/>
+    <sheetView zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1278,8 +1278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fix font in excel file, change to roboto
</commit_message>
<xml_diff>
--- a/docs/01-basics/pie-chart-overview.xlsx
+++ b/docs/01-basics/pie-chart-overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/Documents/developer/github_isaqb/advanced-template/docs/01-basics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09173C1-5A8A-9F47-8274-D52D978FC160}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182FF1B4-E76D-1644-8110-6BB9862D395E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="1900" windowWidth="24560" windowHeight="17660" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1300" yWindow="460" windowWidth="24560" windowHeight="15540" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DE-Grafik" sheetId="3" r:id="rId1"/>
@@ -87,13 +87,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="2">
@@ -118,7 +123,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -139,7 +144,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -472,7 +477,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1204,52 +1209,54 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42" customWidth="1"/>
+    <col min="1" max="1" width="34.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="42" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="1">
         <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>210</v>
       </c>
     </row>
@@ -1257,12 +1264,12 @@
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B7">
+      <c r="B7" s="1">
         <f>SUM(B1:B6)</f>
         <v>960</v>
       </c>
@@ -1278,53 +1285,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42" customWidth="1"/>
+    <col min="1" max="1" width="34.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="42" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="1">
         <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>210</v>
       </c>
     </row>
@@ -1332,12 +1341,12 @@
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B7">
+      <c r="B7" s="1">
         <f>SUM(B1:B6)</f>
         <v>960</v>
       </c>
@@ -1352,127 +1361,130 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView zoomScale="249" zoomScaleNormal="249" zoomScalePageLayoutView="249" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="249" zoomScaleNormal="249" zoomScalePageLayoutView="249" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>15</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <f>B2+C2</f>
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>120</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>0</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <f t="shared" ref="D3:D8" si="0">B3+C3</f>
         <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>300</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>90</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <f t="shared" si="0"/>
         <v>390</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>150</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>90</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <f t="shared" si="0"/>
         <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>60</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>30</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>45</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>0</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>60</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>0</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D10">
+      <c r="D10" s="1">
         <f>SUM(D2:D8)</f>
         <v>960</v>
       </c>

</xml_diff>